<commit_message>
Edited careers, recruitment, fudraising spelling
</commit_message>
<xml_diff>
--- a/src/data/summer20/directors_summer20.xlsx
+++ b/src/data/summer20/directors_summer20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyenokida/Projects/dspuci-website-gatsby/src/data/summer20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5269C9-46A2-E541-B1C0-09FAA1593217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C41F62-6AD8-B24A-B46A-ECFD488EB6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Gaurav Mohan</t>
   </si>
   <si>
-    <t>Fundrasing</t>
-  </si>
-  <si>
     <t>Brian Anderson</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Mohit Shah</t>
+  </si>
+  <si>
+    <t>Fundraising</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +463,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -535,10 +535,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>